<commit_message>
added methods to nvm to read things straight out of flash. The methods currently block if the flash is busy.
also added order numbers to R6_BOM_dk_ab_mous.xlsx and updated final
price for alibaba order.
</commit_message>
<xml_diff>
--- a/Circuit/R6/R6_BOM_dk_ab_mous.xlsx
+++ b/Circuit/R6/R6_BOM_dk_ab_mous.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="266">
   <si>
     <t>RES SMD 1K Ohm 1% 1/16W 0402</t>
   </si>
@@ -802,6 +802,24 @@
   </si>
   <si>
     <t>total</t>
+  </si>
+  <si>
+    <t>dk order</t>
+  </si>
+  <si>
+    <t>mouser order</t>
+  </si>
+  <si>
+    <t>NOO20151216-NO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">julixin electronics </t>
+  </si>
+  <si>
+    <t>alibaba</t>
+  </si>
+  <si>
+    <t>paypal fee for alibaba</t>
   </si>
 </sst>
 </file>
@@ -812,14 +830,21 @@
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00000_);_(&quot;$&quot;* \(#,##0.00000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -903,13 +928,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
@@ -920,23 +945,24 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="3" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="1" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="3" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
@@ -1213,10 +1239,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG63"/>
+  <dimension ref="A1:AH63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC65" sqref="AC65"/>
+    <sheetView tabSelected="1" topLeftCell="J52" workbookViewId="0">
+      <selection activeCell="AC64" sqref="AC64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -6420,7 +6446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:33">
+    <row r="49" spans="1:34">
       <c r="A49" s="10">
         <v>50</v>
       </c>
@@ -6520,7 +6546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:33">
+    <row r="50" spans="1:34">
       <c r="A50" s="10">
         <v>52</v>
       </c>
@@ -6622,7 +6648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:33">
+    <row r="51" spans="1:34">
       <c r="A51" s="10">
         <v>53</v>
       </c>
@@ -6732,7 +6758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:33">
+    <row r="52" spans="1:34">
       <c r="A52" s="10">
         <v>54</v>
       </c>
@@ -6842,7 +6868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:33">
+    <row r="53" spans="1:34">
       <c r="A53" s="10">
         <v>55</v>
       </c>
@@ -6952,7 +6978,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:33">
+    <row r="56" spans="1:34">
+      <c r="Y56" t="s">
+        <v>260</v>
+      </c>
+      <c r="Z56">
+        <v>45070136</v>
+      </c>
       <c r="AB56" t="s">
         <v>256</v>
       </c>
@@ -6973,7 +7005,13 @@
         <v>550.79759999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:33">
+    <row r="57" spans="1:34">
+      <c r="Y57" t="s">
+        <v>261</v>
+      </c>
+      <c r="Z57">
+        <v>9661677</v>
+      </c>
       <c r="AB57" t="s">
         <v>257</v>
       </c>
@@ -6987,7 +7025,16 @@
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:33">
+    <row r="58" spans="1:34">
+      <c r="X58" s="28" t="s">
+        <v>264</v>
+      </c>
+      <c r="Y58" s="28" t="s">
+        <v>263</v>
+      </c>
+      <c r="Z58" s="28" t="s">
+        <v>262</v>
+      </c>
       <c r="AC58" t="s">
         <v>258</v>
       </c>
@@ -6995,7 +7042,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="61" spans="1:33">
+    <row r="61" spans="1:34">
       <c r="AC61">
         <v>88.22</v>
       </c>
@@ -7003,11 +7050,10 @@
         <v>118.07</v>
       </c>
       <c r="AE61">
-        <f>AE56</f>
-        <v>346.5</v>
+        <v>344.5</v>
       </c>
     </row>
-    <row r="62" spans="1:33">
+    <row r="62" spans="1:34">
       <c r="AC62">
         <v>6</v>
       </c>
@@ -7015,16 +7061,22 @@
         <v>7</v>
       </c>
       <c r="AE62">
-        <v>23</v>
+        <v>33</v>
+      </c>
+      <c r="AG62" t="s">
+        <v>265</v>
+      </c>
+      <c r="AH62">
+        <v>18.8</v>
       </c>
     </row>
-    <row r="63" spans="1:33">
+    <row r="63" spans="1:34">
       <c r="AB63" s="27" t="s">
         <v>259</v>
       </c>
       <c r="AC63">
-        <f>SUM(AC61:AE62)</f>
-        <v>588.79</v>
+        <f>SUM(AC61:AE62) + AH62</f>
+        <v>615.58999999999992</v>
       </c>
     </row>
   </sheetData>

</xml_diff>